<commit_message>
vault backup: 2023-06-02 14:26:09
</commit_message>
<xml_diff>
--- a/Data/dividend-q1.xlsx
+++ b/Data/dividend-q1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>JASIF</t>
+  </si>
+  <si>
+    <t>TFFIF</t>
   </si>
   <si>
     <t>WHAIR</t>
@@ -426,7 +429,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -481,7 +484,7 @@
         <v>13338</v>
       </c>
       <c r="F2" s="2">
-        <v>45071</v>
+        <v>45069</v>
       </c>
       <c r="G2" s="2">
         <v>45085</v>
@@ -609,7 +612,7 @@
         <v>26910</v>
       </c>
       <c r="F6" s="2">
-        <v>45069</v>
+        <v>45065</v>
       </c>
       <c r="G6" s="2">
         <v>45084</v>
@@ -629,31 +632,31 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>0.1556</v>
+        <v>0.1032</v>
       </c>
       <c r="C7">
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D7">
-        <v>7780</v>
+        <v>2064</v>
       </c>
       <c r="E7">
-        <v>7002</v>
+        <v>1857.6</v>
       </c>
       <c r="F7" s="2">
-        <v>44995</v>
+        <v>45077</v>
       </c>
       <c r="G7" s="2">
-        <v>45015</v>
+        <v>45096</v>
       </c>
       <c r="H7">
-        <v>435000</v>
+        <v>153000</v>
       </c>
       <c r="I7">
-        <v>1.61</v>
+        <v>1.21</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -661,31 +664,63 @@
         <v>16</v>
       </c>
       <c r="B8">
+        <v>0.1369</v>
+      </c>
+      <c r="C8">
+        <v>50000</v>
+      </c>
+      <c r="D8">
+        <v>6845</v>
+      </c>
+      <c r="E8">
+        <v>6160.5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45068</v>
+      </c>
+      <c r="G8" s="2">
+        <v>45099</v>
+      </c>
+      <c r="H8">
+        <v>435000</v>
+      </c>
+      <c r="I8">
+        <v>1.42</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
         <v>0.1915</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>30000</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>5745</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>5170.5</v>
       </c>
-      <c r="F8" s="2">
-        <v>44993</v>
-      </c>
-      <c r="G8" s="2">
-        <v>45009</v>
-      </c>
-      <c r="H8">
+      <c r="F9" s="2">
+        <v>45069</v>
+      </c>
+      <c r="G9" s="2">
+        <v>45086</v>
+      </c>
+      <c r="H9">
         <v>351000</v>
       </c>
-      <c r="I8">
+      <c r="I9">
         <v>1.47</v>
       </c>
-      <c r="J8">
-        <v>0</v>
+      <c r="J9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>